<commit_message>
1. Write README file 2. Attach the requirements.txt to list all the dependencies for this    assessment 3. Attach shell file with UI automation to run python script 4. Correct the help message
</commit_message>
<xml_diff>
--- a/testcases/warranty_defect.xlsx
+++ b/testcases/warranty_defect.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>SerialNumber</t>
   </si>
@@ -23,12 +23,6 @@
   </si>
   <si>
     <t>186232439</t>
-  </si>
-  <si>
-    <t>186232438</t>
-  </si>
-  <si>
-    <t>186232437</t>
   </si>
   <si>
     <t>186232440</t>
@@ -392,7 +386,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -414,7 +408,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -425,29 +419,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
         <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>